<commit_message>
Precompute fire and drought (#22)
* FloodTIF to Flood

* add risk free rate and  company level npm

* tests docs npm rfr

* better UI

* use brazilian reals

* merge bits of branches

* testdata hpdates

* features ok

* wip pass tests

* tests passes

* testpass

* small fix

* controls
</commit_message>
<xml_diff>
--- a/tests/tests_data/user_input/asset_information.xlsx
+++ b/tests/tests_data/user_input/asset_information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>Company</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Soybean</t>
+  </si>
+  <si>
+    <t>AGRI11</t>
   </si>
   <si>
     <t>Company 3_Asset11</t>
@@ -593,7 +596,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1268,7 +1271,7 @@
         <v>60</v>
       </c>
       <c r="C21" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1293,40 +1296,71 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="4" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="6">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="5">
-        <v>-3.7</v>
-      </c>
-      <c r="G22" s="5">
-        <v>-65.1</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="6"/>
       <c r="L22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="5">
+        <v>-3.7</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-65.1</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SNAPSHOT & Fire weather index and other (#21)
* wip fire

* fixes

* testsdata updated

* notebooks

* wips some tests pass

* fixed land cover not being merged

* bugfixes fire mutliple rows

* change snapshot test to compare company results only

* tests pass ok
no fire tests yet

* use nc in test data to speed up test

* waiting for pre-computations to pass

* ok

* Precompute fire and drought (#22)

* FloodTIF to Flood

* add risk free rate and  company level npm

* tests docs npm rfr

* better UI

* use brazilian reals

* merge bits of branches

* testdata hpdates

* features ok

* wip pass tests

* tests passes

* testpass

* small fix

* controls
</commit_message>
<xml_diff>
--- a/tests/tests_data/user_input/asset_information.xlsx
+++ b/tests/tests_data/user_input/asset_information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>Company</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Soybean</t>
+  </si>
+  <si>
+    <t>AGRI11</t>
   </si>
   <si>
     <t>Company 3_Asset11</t>
@@ -593,7 +596,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1268,7 +1271,7 @@
         <v>60</v>
       </c>
       <c r="C21" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1293,40 +1296,71 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="4" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="5">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="6">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="5">
-        <v>-3.7</v>
-      </c>
-      <c r="G22" s="5">
-        <v>-65.1</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="6"/>
       <c r="L22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="5">
+        <v>-3.7</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-65.1</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>